<commit_message>
made "db:users" n "login" n "add new account"
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_URL一覧.xlsx
+++ b/doc/詳細設計/trip_URL一覧.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05.かたち\かたち→家\00.code\tripList\仕様書\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\data\tripList\仕様書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E12E7F-9B63-452A-AF22-2EE9B27A00C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0592B935-CA25-7640-82FA-5113A96B9079}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>機能</t>
     <rPh sb="0" eb="2">
@@ -95,14 +94,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/account/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/account/add.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/account/pass/</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -433,6 +424,34 @@
     <t>その他</t>
     <rPh sb="2" eb="3">
       <t>タ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/account/new/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/account/new/add.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/account/new/check</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録の確認処理と画面</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガメン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -440,7 +459,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -458,7 +477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,12 +493,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +563,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -574,9 +587,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -909,12 +919,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5737E99-7D71-9749-B142-46F9DFBA2B95}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -926,7 +936,7 @@
     <col min="5" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,7 +950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -954,8 +964,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -968,219 +978,229 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" s="14"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="13"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="12"/>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="12"/>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="13"/>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="12"/>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="13"/>
+      <c r="B12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="13"/>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="6" t="s">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="12"/>
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="13"/>
-      <c r="B13" s="6" t="s">
+      <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="12"/>
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="13"/>
-      <c r="B14" s="8" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="12"/>
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D16" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="12"/>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="12"/>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="12"/>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="12"/>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="13"/>
+      <c r="B21" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="13"/>
-      <c r="B15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="13"/>
-      <c r="B16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="C21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="13"/>
-      <c r="B17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="13"/>
-      <c r="B18" s="6" t="s">
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="13"/>
-      <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="14"/>
-      <c r="B20" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="2"/>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="E17:E21"/>
     <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="A13:A21"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
comp account page 01/19
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_URL一覧.xlsx
+++ b/doc/詳細設計/trip_URL一覧.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="2340" yWindow="1335" windowWidth="13125" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>機能</t>
     <rPh sb="0" eb="2">
@@ -108,10 +103,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/account/pass/check.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ログイン処理</t>
     <rPh sb="4" eb="6">
       <t>ショリ</t>
@@ -119,16 +110,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>アカウント登録処理</t>
-    <rPh sb="5" eb="7">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ショリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ログアウト処理</t>
     <rPh sb="5" eb="7">
       <t>ショリ</t>
@@ -165,44 +146,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/account/pass/pass.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>パスワード再設定画面</t>
-    <rPh sb="8" eb="10">
-      <t>ガメン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>登録情報の照合処理</t>
-    <rPh sb="0" eb="2">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ショウゴウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ショリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/account/pass/update.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>パスワード再設定処理</t>
-    <rPh sb="8" eb="10">
-      <t>ショリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>メニュー</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -440,19 +383,76 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>登録の確認処理と画面</t>
+    <t>/account/pass/update.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/account/pass/update_action.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/account/pass/index_action.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再設定画面</t>
+    <rPh sb="0" eb="3">
+      <t>サイセッテイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録情報の照合</t>
     <rPh sb="0" eb="2">
       <t>トウロク</t>
     </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ショウゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>照合と変更</t>
+    <rPh sb="0" eb="2">
+      <t>ショウゴウ</t>
+    </rPh>
     <rPh sb="3" eb="5">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録の商業と確認</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウギョウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
       <t>カクニン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウント登録</t>
     <rPh sb="5" eb="7">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ガメン</t>
-    </rPh>
+      <t>トウロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>insert into</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>update</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -563,7 +563,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -588,6 +588,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -605,6 +608,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,7 +930,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -965,7 +971,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -979,33 +985,33 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1013,185 +1019,189 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="13"/>
+      <c r="B8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="13"/>
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="13"/>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="14"/>
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" s="12"/>
-      <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="13"/>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="13"/>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="13"/>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" s="12"/>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="13"/>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" s="12"/>
-      <c r="B14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="13"/>
+      <c r="B19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" s="12"/>
-      <c r="B15" s="3" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="13"/>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="14"/>
+      <c r="B21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="12"/>
-      <c r="B18" s="3" t="s">
+      <c r="D21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="12"/>
-      <c r="B20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13"/>
-      <c r="B21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2"/>
     </row>

</xml_diff>

<commit_message>
update URL n DB
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_URL一覧.xlsx
+++ b/doc/詳細設計/trip_URL一覧.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>機能</t>
     <rPh sb="0" eb="2">
@@ -174,33 +174,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>登録画面</t>
-    <rPh sb="0" eb="2">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ガメン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/trip/trip.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>行った、行きたいの更新処理</t>
-    <rPh sb="0" eb="1">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ショリ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -232,16 +206,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>更新画面</t>
-    <rPh sb="0" eb="2">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ガメン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/trip/new.php</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -271,16 +235,6 @@
   </si>
   <si>
     <t>/trip/detail.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>詳細画面</t>
-    <rPh sb="0" eb="2">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ガメン</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -316,16 +270,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>別ページにした方がいい？</t>
-    <rPh sb="0" eb="1">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>検索処理→検索結果画面</t>
     <rPh sb="0" eb="2">
       <t>ケンサク</t>
@@ -342,10 +286,6 @@
     <rPh sb="9" eb="11">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/trip/new_action.php</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -428,19 +368,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>登録の商業と確認</t>
-    <rPh sb="0" eb="2">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ショウギョウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>アカウント登録</t>
     <rPh sb="5" eb="7">
       <t>トウロク</t>
@@ -453,6 +380,92 @@
   </si>
   <si>
     <t>update</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録の照合と確認</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウゴウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/new_action.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/delet_action.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>更新確認の画面</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録確認の画面</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>詳細の画面</t>
+    <rPh sb="0" eb="2">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>削除確認の画面</t>
+    <rPh sb="0" eb="2">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>行った、行きたいの変更処理</t>
+    <rPh sb="0" eb="1">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ショリ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -563,7 +576,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -591,8 +604,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -608,9 +621,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,11 +936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1011,7 +1021,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1021,23 +1031,23 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="13"/>
       <c r="B8" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -1050,13 +1060,13 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13"/>
       <c r="B10" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
@@ -1065,23 +1075,23 @@
     <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="14"/>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
@@ -1096,55 +1106,48 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="13"/>
-      <c r="B14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="13"/>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="13"/>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>38</v>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1153,7 +1156,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="10"/>
@@ -1161,56 +1164,68 @@
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13"/>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13"/>
       <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="13"/>
+      <c r="B21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="14"/>
-      <c r="B21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="6" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="9"/>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="2"/>
+      <c r="D23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E17:E21"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="A13:A21"/>
+    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
comp iframe of fooflemap & add bootstrap css
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_URL一覧.xlsx
+++ b/doc/詳細設計/trip_URL一覧.xlsx
@@ -184,13 +184,13 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/trip/search.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>検索処理</t>
-    <rPh sb="0" eb="2">
-      <t>ケンサク</t>
+    <t>/trip/delet.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>削除処理</t>
+    <rPh sb="0" eb="2">
+      <t>サクジョ</t>
     </rPh>
     <rPh sb="2" eb="4">
       <t>ショリ</t>
@@ -198,13 +198,13 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/trip/delet.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>削除処理</t>
-    <rPh sb="0" eb="2">
-      <t>サクジョ</t>
+    <t>/trip/new.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録処理</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
     </rPh>
     <rPh sb="2" eb="4">
       <t>ショリ</t>
@@ -212,13 +212,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/trip/new.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>登録処理</t>
-    <rPh sb="0" eb="2">
-      <t>トウロク</t>
+    <t>更新処理</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
     </rPh>
     <rPh sb="2" eb="4">
       <t>ショリ</t>
@@ -226,16 +222,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>更新処理</t>
-    <rPh sb="0" eb="2">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/trip/edit.php</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -260,37 +246,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>検索処理→検索結果画面</t>
-    <rPh sb="0" eb="2">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ケッカ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ガメン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/trip/edit_action.php</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>/error.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>エラー処理</t>
-    <rPh sb="3" eb="5">
-      <t>ショリ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -506,6 +466,43 @@
     <rPh sb="7" eb="9">
       <t>ガメン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/back.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>検索状態での戻るボタンの処理</t>
+    <rPh sb="0" eb="2">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ショリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sessionをunsetして一覧画面へ戻る</t>
+    <rPh sb="15" eb="17">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エラーメッセージ</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -550,7 +547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -610,13 +607,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -644,26 +650,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,8 +979,8 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1024,7 +1021,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1038,7 +1035,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +1047,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="12"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1060,11 +1057,11 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1072,29 +1069,29 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1104,41 +1101,41 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1150,137 +1147,137 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="10"/>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="10"/>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="10"/>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="10"/>
+      <c r="B18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="10"/>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="10"/>
+      <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="10"/>
+      <c r="B21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="11"/>
-      <c r="B15" s="3" t="s">
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="11"/>
-      <c r="B16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="10"/>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="10"/>
+      <c r="B23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="11"/>
+      <c r="B24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="11"/>
-      <c r="B17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" s="11"/>
-      <c r="B18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="11"/>
-      <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="11"/>
-      <c r="B21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="11"/>
-      <c r="B22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="11"/>
-      <c r="B23" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1288,8 +1285,8 @@
   <mergeCells count="4">
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A12"/>
-    <mergeCell ref="A13:A23"/>
     <mergeCell ref="E19:E21"/>
+    <mergeCell ref="A13:A24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add header.php... this is common file in trip folder
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_URL一覧.xlsx
+++ b/doc/詳細設計/trip_URL一覧.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>機能</t>
     <rPh sb="0" eb="2">
@@ -246,10 +246,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/trip/edit_action.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/error.php</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -325,14 +321,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>insert into</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>update</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>登録の照合と確認</t>
     <rPh sb="0" eb="2">
       <t>トウロク</t>
@@ -343,10 +331,6 @@
     <rPh sb="6" eb="8">
       <t>カクニン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/trip/new_action.php</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -419,24 +403,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>リンクの後ろにidで区別</t>
-    <rPh sb="4" eb="5">
-      <t>ウシ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>クベツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/trip/edit_add.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/trip/new_add.php</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>登録内容の確認画面</t>
     <rPh sb="0" eb="2">
       <t>トウロク</t>
@@ -503,6 +469,56 @@
   </si>
   <si>
     <t>エラーメッセージ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/new_action.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/edit_action.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/new_check.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/edit_check.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リンクの後ろにidで区別（getで取得）</t>
+    <rPh sb="4" eb="5">
+      <t>ウシ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>クベツ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/trip/header.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>headerページ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>require_onceで呼び出す（ユーザー名をSESSIONしているためphpファイルにする）</t>
+    <rPh sb="13" eb="14">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>メイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -976,11 +992,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1061,7 +1077,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1071,24 +1087,22 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="10"/>
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="10"/>
@@ -1103,10 +1117,10 @@
     <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
       <c r="B10" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
@@ -1115,24 +1129,22 @@
     <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="11"/>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>45</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
@@ -1146,147 +1158,159 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10"/>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="10"/>
+      <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10"/>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="10"/>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="10"/>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="10"/>
+      <c r="B19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="10"/>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10"/>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10"/>
-      <c r="B21" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="10"/>
+      <c r="B22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="10"/>
-      <c r="B22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10"/>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="10"/>
+      <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A24" s="11"/>
-      <c r="B24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A12"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="A13:A24"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A13:A25"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fin... next is check
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_URL一覧.xlsx
+++ b/doc/詳細設計/trip_URL一覧.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>機能</t>
     <rPh sb="0" eb="2">
@@ -505,10 +505,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>headerページ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>require_onceで呼び出す（ユーザー名をSESSIONしているためphpファイルにする）</t>
     <rPh sb="13" eb="14">
       <t>ヨ</t>
@@ -519,6 +515,22 @@
     <rPh sb="22" eb="23">
       <t>メイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/account/header.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>トップのheaderページ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>accountディレクトリのheaderページ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tripディレクトリのheaderページ</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -992,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1052,265 +1064,289 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="11"/>
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="10"/>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="10"/>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="6"/>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="10"/>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
       <c r="B10" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="10"/>
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="10"/>
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="6" t="s">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="11"/>
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="9" t="s">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" s="10"/>
-      <c r="B14" s="3" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="10"/>
+      <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="10"/>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10"/>
-      <c r="B16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="10"/>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="10"/>
-      <c r="B18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="10"/>
-      <c r="B19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="6"/>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10"/>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="10"/>
-      <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="12"/>
+      <c r="B21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="10"/>
-      <c r="B22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="6"/>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10"/>
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10"/>
       <c r="B24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="10"/>
+      <c r="B25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="10"/>
+      <c r="B26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A25" s="11"/>
-      <c r="B25" s="6" t="s">
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="11"/>
+      <c r="B27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="A13:A25"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="A15:A27"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>